<commit_message>
criação dos botoes dinamicos para automações, botao voltar e proximo
</commit_message>
<xml_diff>
--- a/planilhas/automacoes.xlsx
+++ b/planilhas/automacoes.xlsx
@@ -1,33 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,89 +50,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -416,111 +358,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
-    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="1" min="1" max="1"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="2" max="2"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="1" min="3" max="3"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="4" max="4"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="5" max="5"/>
+    <col min="1" max="1" style="1" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="1" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Bom dia</t>
-        </is>
-      </c>
-      <c r="B1" t="n">
-        <v>5</v>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Ar da sala</t>
-        </is>
-      </c>
-      <c r="D1" t="n">
-        <v>23</v>
-      </c>
-      <c r="E1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Boa tarde</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>5</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Tv da sala</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>52</v>
-      </c>
-      <c r="E2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Hora de estudar</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>5</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Ar da cozinha</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>24</v>
-      </c>
-      <c r="E3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Hora do almoço</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>5</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Ar do quarto</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>19</v>
-      </c>
-      <c r="E4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Criação da interface nameauto, melhorias na classe newauto e automações
</commit_message>
<xml_diff>
--- a/planilhas/automacoes.xlsx
+++ b/planilhas/automacoes.xlsx
@@ -1,43 +1,58 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -47,30 +62,98 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -358,22 +441,134 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" style="1" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="1" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="1" max="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="2" max="2"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="3" max="3"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="4" max="4"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="5" max="5"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="6" max="6"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" ht="19.5" customHeight="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>Ar da sala</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>A/C</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="E1" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F1" s="4" t="n"/>
+    </row>
+    <row r="2" ht="19.5" customHeight="1">
+      <c r="A2" s="4" t="inlineStr">
+        <is>
+          <t>Bom dia</t>
+        </is>
+      </c>
+      <c r="B2" s="4" t="inlineStr">
+        <is>
+          <t>tv da sala</t>
+        </is>
+      </c>
+      <c r="C2" s="4" t="inlineStr">
+        <is>
+          <t>Televisor</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="F2" s="4" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="18.75" customHeight="1">
+      <c r="A3" s="4" t="inlineStr">
+        <is>
+          <t>Boa noite</t>
+        </is>
+      </c>
+      <c r="B3" s="4" t="inlineStr">
+        <is>
+          <t>tv da sala</t>
+        </is>
+      </c>
+      <c r="C3" s="4" t="inlineStr">
+        <is>
+          <t>Televisor</t>
+        </is>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Hora de estudar</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>tv da sala</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Televisor</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
corrigindo bugs do botão dinâmico das automações
</commit_message>
<xml_diff>
--- a/planilhas/automacoes.xlsx
+++ b/planilhas/automacoes.xlsx
@@ -16,25 +16,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="11"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
@@ -45,14 +33,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -62,19 +43,10 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
     </xf>
@@ -446,7 +418,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,117 +426,86 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="1" max="1"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="2" max="2"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="3" max="3"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="4" max="4"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="5" max="5"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="6" max="6"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="1" min="1" max="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="1" min="2" max="2"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="1" min="3" max="3"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="4" max="4"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="5" max="5"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="1" min="6" max="6"/>
   </cols>
   <sheetData>
-    <row r="1" ht="19.5" customHeight="1">
-      <c r="A1" s="4" t="inlineStr">
+    <row r="1">
+      <c r="A1" t="inlineStr">
         <is>
           <t>Bom dia</t>
         </is>
       </c>
-      <c r="B1" s="4" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>Ar da sala</t>
         </is>
       </c>
-      <c r="C1" s="4" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>A/C</t>
         </is>
       </c>
-      <c r="D1" s="2" t="n">
+      <c r="D1" t="n">
         <v>23</v>
       </c>
-      <c r="E1" s="3" t="b">
+      <c r="E1" t="b">
         <v>0</v>
       </c>
-      <c r="F1" s="4" t="n"/>
     </row>
-    <row r="2" ht="19.5" customHeight="1">
-      <c r="A2" s="4" t="inlineStr">
+    <row r="2">
+      <c r="A2" t="inlineStr">
         <is>
           <t>Bom dia</t>
         </is>
       </c>
-      <c r="B2" s="4" t="inlineStr">
+      <c r="B2" t="inlineStr">
         <is>
           <t>tv da sala</t>
         </is>
       </c>
-      <c r="C2" s="4" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>Televisor</t>
         </is>
       </c>
-      <c r="D2" s="2" t="n">
+      <c r="D2" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="2" t="n">
-        <v>100</v>
-      </c>
-      <c r="F2" s="4" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="b">
+        <v>0</v>
       </c>
     </row>
-    <row r="3" ht="18.75" customHeight="1">
-      <c r="A3" s="4" t="inlineStr">
-        <is>
-          <t>Boa noite</t>
-        </is>
-      </c>
-      <c r="B3" s="4" t="inlineStr">
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Boa tarde</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>tv da sala</t>
         </is>
       </c>
-      <c r="C3" s="4" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>Televisor</t>
         </is>
       </c>
-      <c r="D3" s="3" t="n">
+      <c r="D3" t="n">
         <v>1</v>
       </c>
-      <c r="E3" s="3" t="n">
+      <c r="E3" t="n">
         <v>0</v>
       </c>
-      <c r="F3" s="4" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Hora de estudar</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>tv da sala</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Televisor</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="b">
+      <c r="F3" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
correções nos botões dinâmicos das automações
</commit_message>
<xml_diff>
--- a/planilhas/automacoes.xlsx
+++ b/planilhas/automacoes.xlsx
@@ -1,33 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -45,87 +49,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
+  <cellXfs count="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -413,103 +349,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
-    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
-  <cols>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="1" min="1" max="1"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="1" min="2" max="2"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="1" min="3" max="3"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="4" max="4"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="5" max="5"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="1" min="6" max="6"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Bom dia</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Ar da sala</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>A/C</t>
-        </is>
-      </c>
-      <c r="D1" t="n">
-        <v>23</v>
-      </c>
-      <c r="E1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Bom dia</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>tv da sala</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Televisor</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Boa tarde</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>tv da sala</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Televisor</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
melhorias na interface e nos botões
</commit_message>
<xml_diff>
--- a/planilhas/automacoes.xlsx
+++ b/planilhas/automacoes.xlsx
@@ -1,37 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -49,19 +45,87 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -349,15 +413,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="1" min="1" max="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="1" min="2" max="2"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="1" min="3" max="3"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="4" max="4"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="5" max="5"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="1" min="6" max="6"/>
+  </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
criada a função que executa as automações
</commit_message>
<xml_diff>
--- a/planilhas/automacoes.xlsx
+++ b/planilhas/automacoes.xlsx
@@ -1,39 +1,81 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>tv</t>
+  </si>
+  <si>
+    <t>Televisor</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -45,87 +87,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="6">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -413,151 +402,103 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
-    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="1" min="1" max="1"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="1" min="2" max="2"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="1" min="3" max="3"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="4" max="4"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="5" max="5"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="1" min="6" max="6"/>
+    <col min="1" max="1" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>tv</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Televisor</t>
-        </is>
-      </c>
-      <c r="D1" t="n">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2">
         <v>4</v>
       </c>
-      <c r="E1" t="n">
+      <c r="E1" s="2">
         <v>65</v>
       </c>
-      <c r="F1" t="b">
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>tv</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Televisor</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="n">
-        <v>58</v>
-      </c>
-      <c r="F2" t="b">
+      <c r="D3" s="2">
         <v>1</v>
       </c>
+      <c r="E3" s="2">
+        <v>49</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>tv</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Televisor</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>3</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" t="b">
-        <v>1</v>
-      </c>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="1"/>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>tv</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Televisor</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" t="n">
-        <v>49</v>
-      </c>
-      <c r="F5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>c</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>d</t>
-        </is>
-      </c>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
corrigidos erros na hora de salvar as automações
</commit_message>
<xml_diff>
--- a/planilhas/automacoes.xlsx
+++ b/planilhas/automacoes.xlsx
@@ -1,81 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>tv</t>
-  </si>
-  <si>
-    <t>Televisor</t>
-  </si>
-  <si>
-    <t>true</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>false</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -87,34 +45,90 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -402,103 +416,174 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="1" min="1" max="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="1" min="2" max="2"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="3" max="3"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="4" max="4"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="5" max="5"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="1" min="6" max="6"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="1" t="s">
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>tv</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Televisor</t>
+        </is>
+      </c>
+      <c r="D1" t="n">
+        <v>4</v>
+      </c>
+      <c r="E1" t="n">
+        <v>100</v>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Lâmpada</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>A/C</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>23</v>
+      </c>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>tv</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Televisor</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>4</v>
+      </c>
+      <c r="E4" t="n">
+        <v>65</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Lâmpada</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>A/C</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>16</v>
+      </c>
+      <c r="E6" t="b">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2">
-        <v>4</v>
-      </c>
-      <c r="E1" s="2">
-        <v>65</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2">
-        <v>3</v>
-      </c>
-      <c r="E2" s="2">
-        <v>0</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="2">
-        <v>1</v>
-      </c>
-      <c r="E3" s="2">
-        <v>49</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
corrigindo erro em executar automações
</commit_message>
<xml_diff>
--- a/planilhas/automacoes.xlsx
+++ b/planilhas/automacoes.xlsx
@@ -1,39 +1,81 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>tv</t>
+  </si>
+  <si>
+    <t>Televisor</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>Lâmpada</t>
+  </si>
+  <si>
+    <t>A/C</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -45,90 +87,37 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="7">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -416,174 +405,135 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
-    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="1" min="1" max="1"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="1" min="2" max="2"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="3" max="3"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="4" max="4"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="5" max="5"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="1" min="6" max="6"/>
+    <col min="1" max="1" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>tv</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Televisor</t>
-        </is>
-      </c>
-      <c r="D1" t="n">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2">
+        <v>100</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="n">
-        <v>100</v>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>true</t>
-        </is>
-      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2">
+        <v>10</v>
+      </c>
+      <c r="E2" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1"/>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>l</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Lâmpada</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="b">
-        <v>0</v>
-      </c>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="2">
+        <v>30</v>
+      </c>
+      <c r="E3" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1"/>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>A/C</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>23</v>
-      </c>
-      <c r="E3" t="b">
-        <v>0</v>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2">
+        <v>4</v>
+      </c>
+      <c r="E4" s="2">
+        <v>65</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>tv</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Televisor</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E4" t="n">
-        <v>65</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>true</t>
-        </is>
-      </c>
+      <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1"/>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>l</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Lâmpada</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>A/C</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="2">
         <v>16</v>
       </c>
-      <c r="E6" t="b">
+      <c r="E6" s="3" t="b">
         <v>1</v>
       </c>
+      <c r="F6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
correções no método de excluir dispositivo
</commit_message>
<xml_diff>
--- a/planilhas/automacoes.xlsx
+++ b/planilhas/automacoes.xlsx
@@ -1,68 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>tv</t>
-  </si>
-  <si>
-    <t>Televisor</t>
-  </si>
-  <si>
-    <t>true</t>
-  </si>
-  <si>
-    <t>l</t>
-  </si>
-  <si>
-    <t>Lâmpada</t>
-  </si>
-  <si>
-    <t>A/C</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -85,39 +56,98 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -405,136 +435,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="1" max="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="2" max="2"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="3" max="3"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="4" max="4"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="5" max="5"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="6" max="6"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2">
-        <v>5</v>
-      </c>
-      <c r="E1" s="2">
-        <v>100</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="2">
-        <v>10</v>
-      </c>
-      <c r="E2" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F2" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="2">
-        <v>30</v>
-      </c>
-      <c r="E3" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F3" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="2">
-        <v>4</v>
-      </c>
-      <c r="E4" s="2">
-        <v>65</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="2">
-        <v>0</v>
-      </c>
-      <c r="E5" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F5" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="2">
-        <v>16</v>
-      </c>
-      <c r="E6" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F6" s="1"/>
-    </row>
+    <row r="1" ht="18.75" customHeight="1"/>
+    <row r="2" ht="18.75" customHeight="1"/>
+    <row r="3" ht="18.75" customHeight="1"/>
+    <row r="4" ht="18.75" customHeight="1"/>
+    <row r="5" ht="18.75" customHeight="1"/>
+    <row r="6" ht="18.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Correção problema de várias planilhas instanciadas
</commit_message>
<xml_diff>
--- a/planilhas/automacoes.xlsx
+++ b/planilhas/automacoes.xlsx
@@ -437,7 +437,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -480,26 +480,69 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Boa tarde</t>
+          <t>Ares</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>t2</t>
+          <t>a1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Televisor</t>
+          <t>A/C</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>2</v>
-      </c>
-      <c r="E2" t="n">
-        <v>68</v>
-      </c>
-      <c r="F2" t="b">
+        <v>18</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Ares</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>a2</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>A/C</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>18</v>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Ares</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>l2</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Lâmpada</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
melhorias nas mensagens de confirmação
</commit_message>
<xml_diff>
--- a/planilhas/automacoes.xlsx
+++ b/planilhas/automacoes.xlsx
@@ -437,13 +437,13 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="1" max="1"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="2" max="2"/>
@@ -460,22 +460,71 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>a1</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>A/C</t>
+        </is>
+      </c>
+      <c r="D1" t="n">
+        <v>26</v>
+      </c>
+      <c r="E1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>t1</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>Televisor</t>
         </is>
       </c>
-      <c r="D1" t="n">
+      <c r="D2" t="n">
         <v>1</v>
       </c>
-      <c r="E1" t="n">
-        <v>69</v>
-      </c>
-      <c r="F1" t="b">
+      <c r="E2" t="n">
         <v>0</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>t1</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Televisor</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modularização dos botoes e comentário
</commit_message>
<xml_diff>
--- a/planilhas/automacoes.xlsx
+++ b/planilhas/automacoes.xlsx
@@ -437,7 +437,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,23 +455,26 @@
     <row r="1" ht="18.75" customHeight="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>c</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>a1</t>
+          <t>t1</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>A/C</t>
+          <t>Televisor</t>
         </is>
       </c>
       <c r="D1" t="n">
-        <v>26</v>
-      </c>
-      <c r="E1" t="b">
+        <v>2</v>
+      </c>
+      <c r="E1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F1" t="b">
         <v>1</v>
       </c>
     </row>
@@ -492,38 +495,12 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="F2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>c</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>t1</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Televisor</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>2</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
modularização dos botoes, retorno de funções, tipagem de variáveis e interfaces
</commit_message>
<xml_diff>
--- a/planilhas/automacoes.xlsx
+++ b/planilhas/automacoes.xlsx
@@ -437,7 +437,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,53 +455,70 @@
     <row r="1" ht="18.75" customHeight="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>c</t>
+          <t>v</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>t1</t>
+          <t>ar2</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Televisor</t>
+          <t>A/C</t>
         </is>
       </c>
       <c r="D1" t="n">
-        <v>2</v>
-      </c>
-      <c r="E1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F1" t="b">
+        <v>30</v>
+      </c>
+      <c r="E1" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>b</t>
+          <t>v</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>t1</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Televisor</t>
+          <t>Lâmpada</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>2</v>
-      </c>
-      <c r="E2" t="n">
-        <v>58</v>
-      </c>
-      <c r="F2" t="b">
-        <v>1</v>
+        <v>100</v>
+      </c>
+      <c r="E2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ae</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>A/C</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>26</v>
+      </c>
+      <c r="E3" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Versão final com seleção de alterações
</commit_message>
<xml_diff>
--- a/planilhas/automacoes.xlsx
+++ b/planilhas/automacoes.xlsx
@@ -437,7 +437,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,75 +452,7 @@
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="5" max="5"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.75" customHeight="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>v</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>ar2</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>A/C</t>
-        </is>
-      </c>
-      <c r="D1" t="n">
-        <v>30</v>
-      </c>
-      <c r="E1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>v</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Lâmpada</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>100</v>
-      </c>
-      <c r="E2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>ae</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>A/C</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>26</v>
-      </c>
-      <c r="E3" t="b">
-        <v>0</v>
-      </c>
-    </row>
+    <row r="1" ht="18.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
melhorias na modularização da classe planilha
</commit_message>
<xml_diff>
--- a/planilhas/automacoes.xlsx
+++ b/planilhas/automacoes.xlsx
@@ -437,13 +437,13 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="1" max="1"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="2" max="2"/>
@@ -452,7 +452,29 @@
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="5" max="5"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.75" customHeight="1"/>
+    <row r="1" ht="18.75" customHeight="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>auto</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>l2</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Lâmpada</t>
+        </is>
+      </c>
+      <c r="D1" t="n">
+        <v>100</v>
+      </c>
+      <c r="E1" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
adicionada o arquivo main.py
</commit_message>
<xml_diff>
--- a/planilhas/automacoes.xlsx
+++ b/planilhas/automacoes.xlsx
@@ -437,13 +437,13 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="1" max="1"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="2" max="2"/>
@@ -452,29 +452,7 @@
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="5" max="5"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.75" customHeight="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>auto</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>l2</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Lâmpada</t>
-        </is>
-      </c>
-      <c r="D1" t="n">
-        <v>100</v>
-      </c>
-      <c r="E1" t="b">
-        <v>0</v>
-      </c>
-    </row>
+    <row r="1" ht="18.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Correções de imports e conexão das interfaces
</commit_message>
<xml_diff>
--- a/planilhas/automacoes.xlsx
+++ b/planilhas/automacoes.xlsx
@@ -437,7 +437,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,7 +452,245 @@
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="5" max="5"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.75" customHeight="1"/>
+    <row r="1" ht="18.75" customHeight="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>auto1</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>ar</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>A/C</t>
+        </is>
+      </c>
+      <c r="D1" t="n">
+        <v>27</v>
+      </c>
+      <c r="E1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>auto2</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ar</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>A/C</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>30</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>auto2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>tv</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Televisor</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" t="n">
+        <v>100</v>
+      </c>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>auto2</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>lamp1</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Lâmpada</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>100</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>AUTO3</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ar</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>A/C</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>16</v>
+      </c>
+      <c r="E5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>AUTO3</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>tv</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Televisor</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>AUTO3</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>lamp1</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Lâmpada</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>auto4</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>ar</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>A/C</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>30</v>
+      </c>
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>auto4</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>tv</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Televisor</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>5</v>
+      </c>
+      <c r="E9" t="n">
+        <v>50</v>
+      </c>
+      <c r="F9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>auto4</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>lamp1</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Lâmpada</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>52</v>
+      </c>
+      <c r="E10" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>